<commit_message>
Tennis Ace- doublefault counter Test
</commit_message>
<xml_diff>
--- a/att/src/main/resources/incidents/Tennis/TennisAceDoublefaultCounter.xlsx
+++ b/att/src/main/resources/incidents/Tennis/TennisAceDoublefaultCounter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmorkhandikar\Desktop\MyExcelsheets for testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmorkhandikar\IdeaProjects\cucumberautomation\att\src\main\resources\incidents\Tennis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB0DC6E-2BA5-4FBC-A0C4-19A650981241}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711E2147-0D45-41EB-BA85-5AAB7B2688D6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{0CAF2721-7CD1-43D6-95B2-B935F5B50283}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="147">
   <si>
     <t>matchTime</t>
   </si>
@@ -444,26 +444,38 @@
     <t>00:40</t>
   </si>
   <si>
-    <t>00:52</t>
-  </si>
-  <si>
     <t>04:55</t>
   </si>
   <si>
+    <t>08:55</t>
+  </si>
+  <si>
+    <t>doublefault</t>
+  </si>
+  <si>
+    <t>00:51</t>
+  </si>
+  <si>
+    <t>30-15</t>
+  </si>
+  <si>
+    <t>00:55</t>
+  </si>
+  <si>
+    <t>40-15</t>
+  </si>
+  <si>
     <t>ace</t>
   </si>
   <si>
-    <t>08:55</t>
-  </si>
-  <si>
-    <t>doublefault</t>
+    <t>tennis_serves_first</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,6 +490,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -509,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
@@ -522,6 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E164CF-D012-422D-ACFE-F9F61FCB1949}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -898,38 +917,38 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
       <c r="G4">
         <v>1</v>
       </c>
@@ -939,40 +958,40 @@
       <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -981,7 +1000,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -1000,37 +1019,37 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="B8" t="s">
         <v>136</v>
@@ -1058,54 +1077,69 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1123,30 +1157,15 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
       <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1160,16 +1179,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -1189,10 +1208,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1218,50 +1237,65 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -1270,7 +1304,7 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -1282,30 +1316,15 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
       <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1318,17 +1337,17 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>31</v>
+      <c r="A19" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -1348,10 +1367,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1377,50 +1396,65 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>4</v>
-      </c>
-      <c r="I22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -1429,7 +1463,7 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
@@ -1441,30 +1475,15 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
       <c r="D24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1477,17 +1496,17 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
+      <c r="A25" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
         <v>34</v>
@@ -1507,10 +1526,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1536,10 +1555,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -1548,7 +1567,7 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F27" t="s">
         <v>16</v>
@@ -1564,25 +1583,40 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
@@ -1600,30 +1634,15 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
       <c r="D30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1637,10 +1656,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
@@ -1666,10 +1685,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -1678,7 +1697,7 @@
         <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
@@ -1694,25 +1713,40 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I33" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -1730,30 +1764,15 @@
         <v>1</v>
       </c>
       <c r="H34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I34" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
       <c r="D35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -1767,10 +1786,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -1796,10 +1815,10 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
@@ -1808,7 +1827,7 @@
         <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F37" t="s">
         <v>16</v>
@@ -1822,7 +1841,65 @@
       <c r="I37" t="s">
         <v>24</v>
       </c>
-      <c r="J37" s="5" t="s">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>